<commit_message>
Updated more filenames and added initial firmware skeleton
</commit_message>
<xml_diff>
--- a/Notes/Pong.0 BOM.xlsx
+++ b/Notes/Pong.0 BOM.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Electronics" sheetId="1" r:id="rId1"/>
     <sheet name="Other" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Goal" localSheetId="1">Other!$J$1</definedName>
@@ -256,12 +255,6 @@
     <t>Capacitor Ceramic 0.1uF 50V 10%</t>
   </si>
   <si>
-    <t>Bill of Materials - BPS - Other</t>
-  </si>
-  <si>
-    <t>Bill of Materials - BPS - Electronics</t>
-  </si>
-  <si>
     <t>Shipping/Carrying Case</t>
   </si>
   <si>
@@ -272,6 +265,12 @@
   </si>
   <si>
     <t>12 1/8 x 9 1/4 x 3"</t>
+  </si>
+  <si>
+    <t>Bill of Materials - Pong.0 - Electronics</t>
+  </si>
+  <si>
+    <t>Bill of Materials - Pong.0 - Other</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1365,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="27" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -5467,7 +5466,7 @@
   <dimension ref="A1:J200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5487,7 +5486,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="27" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -5580,13 +5579,13 @@
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>80</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>82</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="15">
@@ -5604,7 +5603,7 @@
         <v>635</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J6" s="19"/>
     </row>
@@ -9115,16 +9114,4 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Project Log and added ATTiny84A for slider board testing
</commit_message>
<xml_diff>
--- a/Notes/Pong.0 BOM.xlsx
+++ b/Notes/Pong.0 BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="95">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -69,9 +69,6 @@
     <t>SPX29150T-L-5-0/TR</t>
   </si>
   <si>
-    <t>Atmel AVR ATMEGA644</t>
-  </si>
-  <si>
     <t>TO-263-3</t>
   </si>
   <si>
@@ -271,6 +268,42 @@
   </si>
   <si>
     <t>Bill of Materials - Pong.0 - Other</t>
+  </si>
+  <si>
+    <t>Connector FFC 10 Position</t>
+  </si>
+  <si>
+    <t>Cable Flat Flex 10 Position</t>
+  </si>
+  <si>
+    <t>SMD Right Angle</t>
+  </si>
+  <si>
+    <t>2" @ 1mm pitch</t>
+  </si>
+  <si>
+    <t>Connecting Slider Board and Main Board</t>
+  </si>
+  <si>
+    <t>100R10-51B</t>
+  </si>
+  <si>
+    <t>1-84981-0</t>
+  </si>
+  <si>
+    <t>Atmel AVR ATMega644</t>
+  </si>
+  <si>
+    <t>Atmel AVR ATTiny84A</t>
+  </si>
+  <si>
+    <t>ATTINY84A-SSUR</t>
+  </si>
+  <si>
+    <t>14-SOIC</t>
+  </si>
+  <si>
+    <t>Slider Board Controller</t>
   </si>
 </sst>
 </file>
@@ -281,7 +314,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +412,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Lucida Sans Unicode"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -422,7 +460,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -499,6 +537,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1343,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1365,7 +1406,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1384,7 +1425,7 @@
     </row>
     <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -1416,7 +1457,7 @@
       </c>
       <c r="B4" s="14">
         <f>SUM(I6:I200)</f>
-        <v>13014.579999999998</v>
+        <v>14168.139999999998</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1439,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>12</v>
@@ -1465,7 +1506,7 @@
     </row>
     <row r="6" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>10</v>
@@ -1474,7 +1515,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="17">
         <v>7716</v>
@@ -1500,16 +1541,16 @@
     </row>
     <row r="7" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="17">
         <v>500</v>
@@ -1529,22 +1570,22 @@
         <v>450</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="17">
         <v>2385</v>
@@ -1564,20 +1605,20 @@
         <v>4425</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:11" ht="54" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="15">
@@ -1599,16 +1640,16 @@
     </row>
     <row r="10" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="C10" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="D10" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="E10" s="17">
         <v>116496</v>
@@ -1628,22 +1669,22 @@
         <v>38.25</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="23">
         <v>1206</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="17">
         <v>310439</v>
@@ -1663,22 +1704,22 @@
         <v>201</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K11" s="19"/>
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>29</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>30</v>
       </c>
       <c r="C12" s="23">
         <v>1206</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="17">
         <v>56717</v>
@@ -1698,22 +1739,22 @@
         <v>50.5</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="17">
         <v>7417</v>
@@ -1733,22 +1774,22 @@
         <v>16.5</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="23">
         <v>1206</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="17">
         <v>195000</v>
@@ -1768,22 +1809,22 @@
         <v>14.15</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="C15" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="23" t="s">
-        <v>40</v>
-      </c>
       <c r="D15" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="17">
         <v>53903</v>
@@ -1803,22 +1844,22 @@
         <v>8.94</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="17">
         <v>9900</v>
@@ -1838,22 +1879,22 @@
         <v>268.81</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="23" t="s">
-        <v>46</v>
-      </c>
       <c r="D17" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="17">
         <v>88036</v>
@@ -1873,22 +1914,22 @@
         <v>78.649999999999991</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="23" t="s">
-        <v>51</v>
-      </c>
       <c r="D18" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="17">
         <v>2440</v>
@@ -1908,22 +1949,22 @@
         <v>42.63</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>54</v>
-      </c>
       <c r="C19" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="17">
         <v>1436013</v>
@@ -1943,22 +1984,22 @@
         <v>4.47</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K19" s="19"/>
     </row>
     <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="22" t="s">
-        <v>57</v>
-      </c>
       <c r="C20" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E20" s="17">
         <v>586403</v>
@@ -1978,22 +2019,22 @@
         <v>29.9</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>61</v>
-      </c>
       <c r="C21" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="17">
         <v>123608</v>
@@ -2013,17 +2054,17 @@
         <v>35.78</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="17"/>
@@ -2042,65 +2083,113 @@
         <v>1504</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="15"/>
+      <c r="A23" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="17">
+        <v>812</v>
+      </c>
+      <c r="F23" s="15">
+        <v>1</v>
+      </c>
       <c r="G23" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="18"/>
+        <v>500</v>
+      </c>
+      <c r="H23" s="18">
+        <v>1.2</v>
+      </c>
       <c r="I23" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="19"/>
+        <v>600</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="K23" s="19"/>
     </row>
     <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="15"/>
+      <c r="A24" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="17">
+        <v>5099</v>
+      </c>
+      <c r="F24" s="15">
+        <v>2</v>
+      </c>
       <c r="G24" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="18"/>
+        <v>1000</v>
+      </c>
+      <c r="H24" s="18">
+        <v>0.10406</v>
+      </c>
       <c r="I24" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="19"/>
+        <v>104.06</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="15"/>
+      <c r="A25" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="17">
+        <v>1695</v>
+      </c>
+      <c r="F25" s="15">
+        <v>1</v>
+      </c>
       <c r="G25" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="18"/>
+        <v>500</v>
+      </c>
+      <c r="H25" s="18">
+        <v>0.89900000000000002</v>
+      </c>
       <c r="I25" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="19"/>
+        <v>449.5</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>94</v>
+      </c>
       <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -5449,14 +5538,17 @@
     <hyperlink ref="B20" r:id="rId13"/>
     <hyperlink ref="B21" r:id="rId14"/>
     <hyperlink ref="B10" r:id="rId15"/>
+    <hyperlink ref="B23" r:id="rId16"/>
+    <hyperlink ref="B24" r:id="rId17"/>
+    <hyperlink ref="B25" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
   <ignoredErrors>
     <ignoredError sqref="C13 C15:C21" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5486,7 +5578,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -5504,7 +5596,7 @@
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -5553,7 +5645,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -5579,13 +5671,13 @@
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="C6" s="19" t="s">
         <v>79</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>80</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="15">
@@ -5603,7 +5695,7 @@
         <v>635</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J6" s="19"/>
     </row>

</xml_diff>

<commit_message>
Updated BOM and Requirements Document
</commit_message>
<xml_diff>
--- a/Notes/Pong.0 BOM.xlsx
+++ b/Notes/Pong.0 BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Total Qty Needed</t>
   </si>
   <si>
-    <t>ATMEGA644P-20AU</t>
-  </si>
-  <si>
     <t>44-TQFP</t>
   </si>
   <si>
@@ -63,40 +60,10 @@
     <t>Total BOM Parts Cost:</t>
   </si>
   <si>
-    <t>Also available at Newark, Mouser and Verical. Alternately, ATMEGA324P-20AU or ATMEGA164P-20AU are also acceptable</t>
-  </si>
-  <si>
-    <t>SPX29150T-L-5-0/TR</t>
-  </si>
-  <si>
-    <t>TO-263-3</t>
-  </si>
-  <si>
-    <t>AS1107WL</t>
-  </si>
-  <si>
-    <t>24-SOIC</t>
-  </si>
-  <si>
     <t>Default Supplier</t>
   </si>
   <si>
     <t>DigiKey</t>
-  </si>
-  <si>
-    <t>LDO Voltage Regulator</t>
-  </si>
-  <si>
-    <t>Display Driver</t>
-  </si>
-  <si>
-    <t>Battery (Li-Poly 2500mAh)</t>
-  </si>
-  <si>
-    <t>Shenzhen Puchuangyuan Technology Co. Ltd</t>
-  </si>
-  <si>
-    <t>JHY6529127</t>
   </si>
   <si>
     <t>GRM319R71H104KA01D</t>
@@ -105,85 +72,7 @@
     <t>Used for Power Input/Output filtering and Decoupling</t>
   </si>
   <si>
-    <t>Capacitor Ceramic 4.7nF 50V 10%</t>
-  </si>
-  <si>
-    <t>CC1206KRX7R9BB472</t>
-  </si>
-  <si>
-    <t>Used for QMatrix RY line capacitors</t>
-  </si>
-  <si>
-    <t>CC0805DRNPO9BN8R0</t>
-  </si>
-  <si>
-    <t>Used for Crystal loading</t>
-  </si>
-  <si>
-    <t>RC1206JR-071KL</t>
-  </si>
-  <si>
-    <t>0805</t>
-  </si>
-  <si>
-    <t>Resistor 1.0kΩ 1/4W 5%</t>
-  </si>
-  <si>
-    <t>Used for QMatrix X&amp;Y line resistors</t>
-  </si>
-  <si>
-    <t>Resistor 470K OHM 1/4W 5%</t>
-  </si>
-  <si>
-    <t>RC1206JR-07470KL</t>
-  </si>
-  <si>
     <t>1206</t>
-  </si>
-  <si>
-    <t>Used for QMatrix RY line resistors</t>
-  </si>
-  <si>
-    <t>1210</t>
-  </si>
-  <si>
-    <t>NX3225SA-20.000000MHZ</t>
-  </si>
-  <si>
-    <t>AVR Timing</t>
-  </si>
-  <si>
-    <t>TL3315NF160Q</t>
-  </si>
-  <si>
-    <t>4.5mm x 4.5mm</t>
-  </si>
-  <si>
-    <t>AVR Reset</t>
-  </si>
-  <si>
-    <t>Switch Tactile SPST-NO 0.05A 15V</t>
-  </si>
-  <si>
-    <t>Crystal 20 MHZ 8pF</t>
-  </si>
-  <si>
-    <t>LB3218T330K</t>
-  </si>
-  <si>
-    <t>1207</t>
-  </si>
-  <si>
-    <t>AVR Analog Reference Filtering</t>
-  </si>
-  <si>
-    <t>Resistor 10kΩ 1/4W 5%</t>
-  </si>
-  <si>
-    <t>RC1206JR-0710KL</t>
-  </si>
-  <si>
-    <t>Pull-up for Slave Select on AS1107 and for Reset on AVR</t>
   </si>
   <si>
     <t>LED Red Diffused</t>
@@ -207,18 +96,6 @@
     <t xml:space="preserve"> Projects and Stuff LLC - http://www.projectsandstuff.com</t>
   </si>
   <si>
-    <t>Also available at DigiKey, Verical, Arrow, and Mouser</t>
-  </si>
-  <si>
-    <t>Future Electronics</t>
-  </si>
-  <si>
-    <t>austria microsystems</t>
-  </si>
-  <si>
-    <t>Also available at Future Electronics, and DigiKey, but buying direct saves over a dollar each</t>
-  </si>
-  <si>
     <t>PLCC-6 RGB LED</t>
   </si>
   <si>
@@ -228,25 +105,10 @@
     <t>5mm x 5mm</t>
   </si>
   <si>
-    <t>Capacitor Ceramic 10uF 10V Y5V</t>
-  </si>
-  <si>
-    <t>C3216Y5V1A106Z/0.85</t>
-  </si>
-  <si>
-    <t>3.2mm x 1.6mm</t>
-  </si>
-  <si>
     <t>Digikey</t>
   </si>
   <si>
     <t>Used for Supply Filtering (Input and Output). Low ESR</t>
-  </si>
-  <si>
-    <t>Inductor 33uH 10%</t>
-  </si>
-  <si>
-    <t>Capacitor Ceramic 8pF 50V</t>
   </si>
   <si>
     <t>Capacitor Ceramic 0.1uF 50V 10%</t>
@@ -270,43 +132,79 @@
     <t>Bill of Materials - Pong.0 - Other</t>
   </si>
   <si>
-    <t>Connector FFC 10 Position</t>
+    <t>KiCad Footprint</t>
   </si>
   <si>
-    <t>Cable Flat Flex 10 Position</t>
+    <t>TPS61240DRVT</t>
   </si>
   <si>
-    <t>SMD Right Angle</t>
+    <t>5V 0.45A Boost Regulator</t>
   </si>
   <si>
-    <t>2" @ 1mm pitch</t>
+    <t>6-WDFN</t>
   </si>
   <si>
-    <t>Connecting Slider Board and Main Board</t>
+    <t>5V Power for LEDs and Drivers</t>
   </si>
   <si>
-    <t>100R10-51B</t>
+    <t>64 LED Driver</t>
   </si>
   <si>
-    <t>1-84981-0</t>
+    <t>Capacitor Aluminum 10uF</t>
   </si>
   <si>
-    <t>Atmel AVR ATMega644</t>
+    <t>Level Translator</t>
   </si>
   <si>
-    <t>Atmel AVR ATTiny84A</t>
+    <t>NVT2006PW,118</t>
   </si>
   <si>
-    <t>ATTINY84A-SSUR</t>
+    <t>16-TSSOP</t>
   </si>
   <si>
-    <t>14-SOIC</t>
+    <t>Part Cost Per Board:</t>
   </si>
   <si>
-    <t>Slider Board Controller</t>
+    <t>SPI/I2C translation for the LED Drivers</t>
   </si>
   <si>
-    <t>KiCad Footprint</t>
+    <t>AS1116-BSST</t>
+  </si>
+  <si>
+    <t>24-QSOP</t>
+  </si>
+  <si>
+    <t>SPI LED Driver</t>
+  </si>
+  <si>
+    <t>ZX62WRD-B-5PC</t>
+  </si>
+  <si>
+    <t>USB Connector</t>
+  </si>
+  <si>
+    <t>Water Resistant Micro B USB Connector</t>
+  </si>
+  <si>
+    <t>USB Micro B</t>
+  </si>
+  <si>
+    <t>CC2500RTKR</t>
+  </si>
+  <si>
+    <t>RF Transceiver</t>
+  </si>
+  <si>
+    <t>20-VFQFN</t>
+  </si>
+  <si>
+    <t>2.4GHz Transceiver</t>
+  </si>
+  <si>
+    <t>ATXMEGA16A4U-AUR</t>
+  </si>
+  <si>
+    <t>Atmel AVR XMEGA16A4U</t>
   </si>
 </sst>
 </file>
@@ -463,7 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -544,31 +442,24 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Lucida Sans Unicode"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -975,6 +866,25 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="9"/>
+        <color theme="1"/>
+        <name val="Lucida Sans Unicode"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
         <color theme="1" tint="0.14996795556505021"/>
         <name val="Lucida Sans Unicode"/>
         <scheme val="none"/>
@@ -1071,48 +981,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A5:L200" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="A5:L200"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A4:L199" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A4:L199"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Description" dataDxfId="23"/>
     <tableColumn id="2" name="Mfg Part #" dataDxfId="22"/>
     <tableColumn id="3" name="Package" dataDxfId="21"/>
-    <tableColumn id="12" name="KiCad Footprint" dataDxfId="0"/>
-    <tableColumn id="5" name="Default Supplier" dataDxfId="20"/>
-    <tableColumn id="10" name="Supplier On Hand" dataDxfId="19"/>
-    <tableColumn id="4" name="Qty per board" dataDxfId="18"/>
-    <tableColumn id="6" name="Total Qty Needed" dataDxfId="17">
+    <tableColumn id="12" name="KiCad Footprint" dataDxfId="20"/>
+    <tableColumn id="5" name="Default Supplier" dataDxfId="19"/>
+    <tableColumn id="10" name="Supplier On Hand" dataDxfId="18"/>
+    <tableColumn id="4" name="Qty per board" dataDxfId="17"/>
+    <tableColumn id="6" name="Total Qty Needed" dataDxfId="16">
       <calculatedColumnFormula>SUM(Table4[[#This Row],[Qty per board]]*Goal)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Price per part at Qty" dataDxfId="16"/>
-    <tableColumn id="7" name="Total Price" dataDxfId="15">
-      <calculatedColumnFormula>SUM(I6*H6)</calculatedColumnFormula>
+    <tableColumn id="11" name="Price per part at Qty" dataDxfId="15"/>
+    <tableColumn id="7" name="Total Price" dataDxfId="14">
+      <calculatedColumnFormula>SUM(I5*H5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Notes" dataDxfId="14"/>
-    <tableColumn id="9" name="Part References" dataDxfId="13"/>
+    <tableColumn id="8" name="Notes" dataDxfId="13"/>
+    <tableColumn id="9" name="Part References" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="Projects and Stuff" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table42" displayName="Table42" ref="A5:J200" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table42" displayName="Table42" ref="A5:J200" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A5:J200"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Description" dataDxfId="10"/>
-    <tableColumn id="2" name="Mfg Part #" dataDxfId="9"/>
-    <tableColumn id="5" name="Default Supplier" dataDxfId="8"/>
-    <tableColumn id="10" name="Supplier On Hand" dataDxfId="7"/>
-    <tableColumn id="4" name="Qty per board" dataDxfId="6"/>
-    <tableColumn id="6" name="Total Qty Needed" dataDxfId="5">
+    <tableColumn id="1" name="Description" dataDxfId="9"/>
+    <tableColumn id="2" name="Mfg Part #" dataDxfId="8"/>
+    <tableColumn id="5" name="Default Supplier" dataDxfId="7"/>
+    <tableColumn id="10" name="Supplier On Hand" dataDxfId="6"/>
+    <tableColumn id="4" name="Qty per board" dataDxfId="5"/>
+    <tableColumn id="6" name="Total Qty Needed" dataDxfId="4">
       <calculatedColumnFormula>SUM(Table42[[#This Row],[Qty per board]]*Goal)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Price per part at Qty" dataDxfId="4"/>
-    <tableColumn id="7" name="Total Price" dataDxfId="3">
+    <tableColumn id="11" name="Price per part at Qty" dataDxfId="3"/>
+    <tableColumn id="7" name="Total Price" dataDxfId="2">
       <calculatedColumnFormula>SUM(G6*F6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Notes" dataDxfId="2"/>
-    <tableColumn id="9" name="Part References" dataDxfId="1"/>
+    <tableColumn id="8" name="Notes" dataDxfId="1"/>
+    <tableColumn id="9" name="Part References" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Projects and Stuff" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1405,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L200"/>
+  <dimension ref="A1:L199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1430,7 +1340,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1450,7 +1360,7 @@
     </row>
     <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -1464,93 +1374,118 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+    <row r="3" spans="1:12" s="33" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="31">
+        <f>SUM(J5:J199)</f>
+        <v>8763.8849999999984</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="31">
+        <f>B3/Goal</f>
+        <v>17.527769999999997</v>
+      </c>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="14">
-        <f>SUM(J6:J200)</f>
-        <v>14168.139999999998</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="17">
+        <v>3483</v>
+      </c>
+      <c r="G5" s="15">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="H5" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I5" s="18">
+        <v>2.0038999999999998</v>
+      </c>
+      <c r="J5" s="24">
+        <f>SUM(I5*H5)</f>
+        <v>1001.9499999999999</v>
+      </c>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>10</v>
+        <v>44</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F6" s="17">
-        <v>7716</v>
+        <v>7348</v>
       </c>
       <c r="G6" s="15">
         <v>1</v>
@@ -1560,687 +1495,525 @@
         <v>500</v>
       </c>
       <c r="I6" s="18">
-        <v>4.5119999999999996</v>
+        <v>0.49</v>
       </c>
       <c r="J6" s="24">
         <f>SUM(I6*H6)</f>
-        <v>2256</v>
+        <v>245</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>15</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B7" s="20"/>
       <c r="C7" s="23" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D7" s="23"/>
-      <c r="E7" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="17">
-        <v>500</v>
-      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="15">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="H7" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
+        <v>23500</v>
       </c>
       <c r="I7" s="18">
-        <v>0.9</v>
+        <v>0.03</v>
       </c>
       <c r="J7" s="24">
         <f>SUM(I7*H7)</f>
-        <v>450</v>
+        <v>705</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="23"/>
+        <v>43</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="17">
-        <v>2385</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F8" s="17"/>
       <c r="G8" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H8" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1500</v>
-      </c>
-      <c r="I8" s="18">
-        <v>2.95</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="I8" s="18"/>
       <c r="J8" s="24">
-        <f>SUM(I8*H8)</f>
-        <v>4425</v>
+        <f t="shared" ref="J8:J68" si="0">SUM(I8*H8)</f>
+        <v>0</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:12" ht="54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="23"/>
+        <v>30</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="23">
+        <v>1206</v>
+      </c>
       <c r="D9" s="23"/>
       <c r="E9" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="17"/>
+        <v>14</v>
+      </c>
+      <c r="F9" s="17">
+        <v>425577</v>
+      </c>
       <c r="G9" s="15">
+        <v>30</v>
+      </c>
+      <c r="H9" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>15000</v>
+      </c>
+      <c r="I9" s="18">
+        <v>2.01E-2</v>
+      </c>
+      <c r="J9" s="24">
+        <f t="shared" si="0"/>
+        <v>301.5</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="19"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="17">
+        <v>46342</v>
+      </c>
+      <c r="G10" s="15">
         <v>1</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H10" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>500</v>
       </c>
-      <c r="I9" s="18">
-        <v>7.18</v>
-      </c>
-      <c r="J9" s="24">
-        <f t="shared" ref="J9:J69" si="0">SUM(I9*H9)</f>
-        <v>3590</v>
-      </c>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-    </row>
-    <row r="10" spans="1:12" ht="27" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="17">
-        <v>116496</v>
-      </c>
-      <c r="G10" s="15">
-        <v>2</v>
-      </c>
-      <c r="H10" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
-      </c>
       <c r="I10" s="18">
-        <v>3.8249999999999999E-2</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="J10" s="24">
         <f t="shared" si="0"/>
-        <v>38.25</v>
+        <v>28.75</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="23">
-        <v>1206</v>
+        <v>23</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F11" s="17">
-        <v>310439</v>
+        <v>84494</v>
       </c>
       <c r="G11" s="15">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="H11" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>15000</v>
+        <v>500</v>
       </c>
       <c r="I11" s="18">
-        <v>1.34E-2</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="J11" s="24">
         <f t="shared" si="0"/>
-        <v>201</v>
+        <v>28.75</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="23">
-        <v>1206</v>
+        <v>38</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F12" s="17">
-        <v>56717</v>
+        <v>51750</v>
       </c>
       <c r="G12" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H12" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="I12" s="18">
-        <v>2.5250000000000002E-2</v>
+        <v>0.9425</v>
       </c>
       <c r="J12" s="24">
         <f t="shared" si="0"/>
-        <v>50.5</v>
+        <v>471.25</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F13" s="17">
-        <v>7417</v>
+        <v>12727</v>
       </c>
       <c r="G13" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H13" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="I13" s="18">
-        <v>1.6500000000000001E-2</v>
+        <v>3.1905899999999998</v>
       </c>
       <c r="J13" s="24">
         <f t="shared" si="0"/>
-        <v>16.5</v>
+        <v>4785.8849999999993</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="L13" s="19"/>
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="23">
-        <v>1206</v>
+        <v>52</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F14" s="17">
-        <v>195000</v>
+        <v>5213</v>
       </c>
       <c r="G14" s="15">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H14" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="I14" s="18">
-        <v>2.8300000000000001E-3</v>
+        <v>0.83160000000000001</v>
       </c>
       <c r="J14" s="24">
         <f t="shared" si="0"/>
-        <v>14.15</v>
+        <v>415.8</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="L14" s="19"/>
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F15" s="17">
-        <v>53903</v>
+        <v>15533</v>
       </c>
       <c r="G15" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H15" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="I15" s="18">
-        <v>4.47E-3</v>
+        <v>1.56</v>
       </c>
       <c r="J15" s="24">
         <f t="shared" si="0"/>
-        <v>8.94</v>
+        <v>780</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>41</v>
-      </c>
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="23"/>
-      <c r="E16" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="17">
-        <v>9900</v>
-      </c>
-      <c r="G16" s="15">
-        <v>1</v>
-      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I16" s="18">
-        <v>0.53761999999999999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I16" s="18"/>
       <c r="J16" s="24">
         <f t="shared" si="0"/>
-        <v>268.81</v>
-      </c>
-      <c r="K16" s="19" t="s">
-        <v>43</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K16" s="19"/>
       <c r="L16" s="19"/>
     </row>
     <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>45</v>
-      </c>
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="23"/>
-      <c r="E17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="17">
-        <v>88036</v>
-      </c>
-      <c r="G17" s="15">
-        <v>1</v>
-      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="15"/>
       <c r="H17" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I17" s="18">
-        <v>0.1573</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I17" s="18"/>
       <c r="J17" s="24">
         <f t="shared" si="0"/>
-        <v>78.649999999999991</v>
-      </c>
-      <c r="K17" s="19" t="s">
-        <v>46</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K17" s="19"/>
       <c r="L17" s="19"/>
     </row>
     <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>50</v>
-      </c>
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="23"/>
-      <c r="E18" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="17">
-        <v>2440</v>
-      </c>
-      <c r="G18" s="15">
-        <v>1</v>
-      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="15"/>
       <c r="H18" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I18" s="18">
-        <v>8.5260000000000002E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I18" s="18"/>
       <c r="J18" s="24">
         <f t="shared" si="0"/>
-        <v>42.63</v>
-      </c>
-      <c r="K18" s="19" t="s">
-        <v>51</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K18" s="19"/>
       <c r="L18" s="19"/>
     </row>
-    <row r="19" spans="1:12" ht="27" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>39</v>
-      </c>
+    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="23"/>
-      <c r="E19" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="17">
-        <v>1436013</v>
-      </c>
-      <c r="G19" s="15">
-        <v>2</v>
-      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="15"/>
       <c r="H19" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
-      </c>
-      <c r="I19" s="18">
-        <v>4.47E-3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I19" s="18"/>
       <c r="J19" s="24">
         <f t="shared" si="0"/>
-        <v>4.47</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>54</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K19" s="19"/>
       <c r="L19" s="19"/>
     </row>
     <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>39</v>
-      </c>
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="23"/>
-      <c r="E20" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="17">
-        <v>586403</v>
-      </c>
-      <c r="G20" s="15">
-        <v>1</v>
-      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="15"/>
       <c r="H20" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I20" s="18">
-        <v>5.9799999999999999E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I20" s="18"/>
       <c r="J20" s="24">
         <f t="shared" si="0"/>
-        <v>29.9</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>57</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K20" s="19"/>
       <c r="L20" s="19"/>
     </row>
     <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>39</v>
-      </c>
+      <c r="A21" s="21"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="23"/>
-      <c r="E21" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="17">
-        <v>123608</v>
-      </c>
-      <c r="G21" s="15">
-        <v>1</v>
-      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="15"/>
       <c r="H21" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I21" s="18">
-        <v>7.1559999999999999E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I21" s="18"/>
       <c r="J21" s="24">
         <f t="shared" si="0"/>
-        <v>35.78</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>58</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K21" s="19"/>
       <c r="L21" s="19"/>
     </row>
     <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="23"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="19"/>
       <c r="F22" s="17"/>
-      <c r="G22" s="15">
-        <v>47</v>
-      </c>
+      <c r="G22" s="15"/>
       <c r="H22" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>23500</v>
-      </c>
-      <c r="I22" s="18">
-        <v>6.4000000000000001E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I22" s="18"/>
       <c r="J22" s="24">
         <f t="shared" si="0"/>
-        <v>1504</v>
-      </c>
-      <c r="K22" s="19" t="s">
-        <v>67</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K22" s="19"/>
       <c r="L22" s="19"/>
     </row>
     <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="17">
-        <v>812</v>
-      </c>
-      <c r="G23" s="15">
-        <v>1</v>
-      </c>
+      <c r="A23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="15"/>
       <c r="H23" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I23" s="18">
-        <v>1.2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I23" s="18"/>
       <c r="J23" s="24">
         <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-      <c r="K23" s="19" t="s">
-        <v>87</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K23" s="19"/>
       <c r="L23" s="19"/>
     </row>
     <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>85</v>
-      </c>
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="23"/>
-      <c r="E24" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="17">
-        <v>5099</v>
-      </c>
-      <c r="G24" s="15">
-        <v>2</v>
-      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="15"/>
       <c r="H24" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1000</v>
-      </c>
-      <c r="I24" s="18">
-        <v>0.10406</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I24" s="18"/>
       <c r="J24" s="24">
         <f t="shared" si="0"/>
-        <v>104.06</v>
-      </c>
-      <c r="K24" s="19" t="s">
-        <v>87</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K24" s="19"/>
       <c r="L24" s="19"/>
     </row>
     <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>93</v>
-      </c>
+      <c r="A25" s="21"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="23"/>
-      <c r="E25" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="17">
-        <v>1695</v>
-      </c>
-      <c r="G25" s="15">
-        <v>1</v>
-      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="15"/>
       <c r="H25" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I25" s="18">
-        <v>0.89900000000000002</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I25" s="18"/>
       <c r="J25" s="24">
         <f t="shared" si="0"/>
-        <v>449.5</v>
-      </c>
-      <c r="K25" s="19" t="s">
-        <v>94</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K25" s="19"/>
       <c r="L25" s="19"/>
     </row>
     <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -3117,7 +2890,7 @@
       </c>
       <c r="I69" s="18"/>
       <c r="J69" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J69:J132" si="1">SUM(I69*H69)</f>
         <v>0</v>
       </c>
       <c r="K69" s="19"/>
@@ -3137,7 +2910,7 @@
       </c>
       <c r="I70" s="18"/>
       <c r="J70" s="24">
-        <f t="shared" ref="J70:J133" si="1">SUM(I70*H70)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K70" s="19"/>
@@ -4397,7 +4170,7 @@
       </c>
       <c r="I133" s="18"/>
       <c r="J133" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J133:J196" si="2">SUM(I133*H133)</f>
         <v>0</v>
       </c>
       <c r="K133" s="19"/>
@@ -4417,7 +4190,7 @@
       </c>
       <c r="I134" s="18"/>
       <c r="J134" s="24">
-        <f t="shared" ref="J134:J197" si="2">SUM(I134*H134)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K134" s="19"/>
@@ -5677,7 +5450,7 @@
       </c>
       <c r="I197" s="18"/>
       <c r="J197" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J197:J199" si="3">SUM(I197*H197)</f>
         <v>0</v>
       </c>
       <c r="K197" s="19"/>
@@ -5697,7 +5470,7 @@
       </c>
       <c r="I198" s="18"/>
       <c r="J198" s="24">
-        <f t="shared" ref="J198:J200" si="3">SUM(I198*H198)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K198" s="19"/>
@@ -5723,26 +5496,6 @@
       <c r="K199" s="19"/>
       <c r="L199" s="19"/>
     </row>
-    <row r="200" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A200" s="21"/>
-      <c r="B200" s="20"/>
-      <c r="C200" s="23"/>
-      <c r="D200" s="23"/>
-      <c r="E200" s="19"/>
-      <c r="F200" s="17"/>
-      <c r="G200" s="15"/>
-      <c r="H200" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I200" s="18"/>
-      <c r="J200" s="24">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K200" s="19"/>
-      <c r="L200" s="19"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:J1"/>
@@ -5750,31 +5503,17 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2:J2" r:id="rId1" display=" Projects and Stuff LLC - http://ww.projectsandstuff.com"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B12" r:id="rId5"/>
-    <hyperlink ref="B11" r:id="rId6"/>
-    <hyperlink ref="B13" r:id="rId7"/>
-    <hyperlink ref="B14" r:id="rId8"/>
-    <hyperlink ref="B15" r:id="rId9"/>
-    <hyperlink ref="B16" r:id="rId10"/>
-    <hyperlink ref="B17" r:id="rId11"/>
-    <hyperlink ref="B18" r:id="rId12"/>
-    <hyperlink ref="B20" r:id="rId13"/>
-    <hyperlink ref="B21" r:id="rId14"/>
-    <hyperlink ref="B10" r:id="rId15"/>
-    <hyperlink ref="B23" r:id="rId16"/>
-    <hyperlink ref="B24" r:id="rId17"/>
-    <hyperlink ref="B25" r:id="rId18"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B13" r:id="rId5"/>
+    <hyperlink ref="B14" r:id="rId6"/>
+    <hyperlink ref="B15" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
-  <ignoredErrors>
-    <ignoredError sqref="C13 C15:C21" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5804,7 +5543,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -5822,7 +5561,7 @@
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -5848,7 +5587,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="14">
         <f>SUM(H6:H200)</f>
@@ -5871,10 +5610,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
@@ -5897,13 +5636,13 @@
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="15">
@@ -5921,7 +5660,7 @@
         <v>635</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="J6" s="19"/>
     </row>

</xml_diff>

<commit_message>
Updated BOM and Schematic with significant components
</commit_message>
<xml_diff>
--- a/Notes/Pong.0 BOM.xlsx
+++ b/Notes/Pong.0 BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -72,13 +72,7 @@
     <t>Used for Power Input/Output filtering and Decoupling</t>
   </si>
   <si>
-    <t>1206</t>
-  </si>
-  <si>
     <t>LED Red Diffused</t>
-  </si>
-  <si>
-    <t>LH N974-KN-1</t>
   </si>
   <si>
     <t>Power Indicator</t>
@@ -205,6 +199,33 @@
   </si>
   <si>
     <t>Atmel AVR XMEGA16A4U</t>
+  </si>
+  <si>
+    <t>ABM8G-26.000MHZ-4Y-T3</t>
+  </si>
+  <si>
+    <t>4-SMD</t>
+  </si>
+  <si>
+    <t>Reference Crystal for RF Chip CC2500</t>
+  </si>
+  <si>
+    <t>26 MHz Crystal</t>
+  </si>
+  <si>
+    <t>24-VFQFN</t>
+  </si>
+  <si>
+    <t>BQ24163RGET</t>
+  </si>
+  <si>
+    <t>Battery Manager/Charger</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>LH R974-LP-1</t>
   </si>
 </sst>
 </file>
@@ -436,12 +457,6 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -453,6 +468,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1318,7 +1339,7 @@
   <dimension ref="A1:L199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1339,18 +1360,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="A1" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
       <c r="K1" s="8" t="s">
         <v>4</v>
       </c>
@@ -1359,44 +1380,44 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="A2" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" s="33" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:12" s="31" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="29">
         <f>SUM(J5:J199)</f>
-        <v>8763.8849999999984</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="31">
+        <v>10322.834999999999</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="29">
         <f>B3/Goal</f>
-        <v>17.527769999999997</v>
-      </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
+        <v>20.645669999999999</v>
+      </c>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -1409,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -1438,10 +1459,10 @@
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>10</v>
@@ -1472,13 +1493,13 @@
     </row>
     <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>44</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>46</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="19" t="s">
@@ -1502,17 +1523,17 @@
         <v>245</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="19"/>
@@ -1532,19 +1553,19 @@
         <v>705</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
       <c r="E8" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="15">
@@ -1560,13 +1581,13 @@
         <v>0</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>15</v>
@@ -1602,20 +1623,20 @@
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="17">
-        <v>46342</v>
+        <v>43194</v>
       </c>
       <c r="G10" s="15">
         <v>1</v>
@@ -1625,33 +1646,33 @@
         <v>500</v>
       </c>
       <c r="I10" s="18">
-        <v>5.7500000000000002E-2</v>
+        <v>4.3700000000000003E-2</v>
       </c>
       <c r="J10" s="24">
         <f t="shared" si="0"/>
-        <v>28.75</v>
+        <v>21.85</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="17">
-        <v>84494</v>
+        <v>94327</v>
       </c>
       <c r="G11" s="15">
         <v>1</v>
@@ -1661,26 +1682,26 @@
         <v>500</v>
       </c>
       <c r="I11" s="18">
-        <v>5.7500000000000002E-2</v>
+        <v>4.3700000000000003E-2</v>
       </c>
       <c r="J11" s="24">
         <f t="shared" si="0"/>
-        <v>28.75</v>
+        <v>21.85</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>38</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>40</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="19" t="s">
@@ -1704,19 +1725,19 @@
         <v>471.25</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="19" t="s">
@@ -1740,19 +1761,19 @@
         <v>4785.8849999999993</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L13" s="19"/>
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>53</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>55</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="19" t="s">
@@ -1776,19 +1797,19 @@
         <v>415.8</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L14" s="19"/>
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>56</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>58</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="19" t="s">
@@ -1812,46 +1833,76 @@
         <v>780</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
+      <c r="A16" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
       <c r="D16" s="23"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="15"/>
+      <c r="E16" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="17">
+        <v>6517</v>
+      </c>
+      <c r="G16" s="15">
+        <v>1</v>
+      </c>
       <c r="H16" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="18"/>
+        <v>500</v>
+      </c>
+      <c r="I16" s="18">
+        <v>0.51300000000000001</v>
+      </c>
       <c r="J16" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="19"/>
+        <v>256.5</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>62</v>
+      </c>
       <c r="L16" s="19"/>
     </row>
     <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
+      <c r="A17" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>64</v>
+      </c>
       <c r="D17" s="23"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="15"/>
+      <c r="E17" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="17">
+        <v>706</v>
+      </c>
+      <c r="G17" s="15">
+        <v>1</v>
+      </c>
       <c r="H17" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="18"/>
+        <v>500</v>
+      </c>
+      <c r="I17" s="18">
+        <v>2.6324999999999998</v>
+      </c>
       <c r="J17" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1316.25</v>
       </c>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
@@ -5509,11 +5560,15 @@
     <hyperlink ref="B13" r:id="rId5"/>
     <hyperlink ref="B14" r:id="rId6"/>
     <hyperlink ref="B15" r:id="rId7"/>
+    <hyperlink ref="B16" r:id="rId8"/>
+    <hyperlink ref="B17" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B10" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5542,16 +5597,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="A1" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
       <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
@@ -5560,16 +5615,16 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="A2" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
@@ -5636,13 +5691,13 @@
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>33</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="15">
@@ -5660,7 +5715,7 @@
         <v>635</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J6" s="19"/>
     </row>

</xml_diff>

<commit_message>
Added items from Schematics to BOM.
</commit_message>
<xml_diff>
--- a/Notes/Pong.0 BOM.xlsx
+++ b/Notes/Pong.0 BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>LH R974-LP-1</t>
+  </si>
+  <si>
+    <t>IP4234CZ6,125</t>
+  </si>
+  <si>
+    <t>6-TSOP</t>
+  </si>
+  <si>
+    <t>USB ESD Protection</t>
   </si>
 </sst>
 </file>
@@ -1339,7 +1348,7 @@
   <dimension ref="A1:L199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1401,7 +1410,7 @@
       </c>
       <c r="B3" s="29">
         <f>SUM(J5:J199)</f>
-        <v>10322.834999999999</v>
+        <v>10430.664999999999</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>45</v>
@@ -1409,7 +1418,7 @@
       <c r="D3" s="30"/>
       <c r="E3" s="29">
         <f>B3/Goal</f>
-        <v>20.645669999999999</v>
+        <v>20.861329999999999</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -1908,21 +1917,35 @@
       <c r="L17" s="19"/>
     </row>
     <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
+      <c r="A18" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>70</v>
+      </c>
       <c r="D18" s="23"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="15"/>
+      <c r="E18" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="17">
+        <v>8164</v>
+      </c>
+      <c r="G18" s="15">
+        <v>1</v>
+      </c>
       <c r="H18" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="18"/>
+        <v>500</v>
+      </c>
+      <c r="I18" s="18">
+        <v>0.21565999999999999</v>
+      </c>
       <c r="J18" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>107.83</v>
       </c>
       <c r="K18" s="19"/>
       <c r="L18" s="19"/>
@@ -5564,11 +5587,12 @@
     <hyperlink ref="B17" r:id="rId9"/>
     <hyperlink ref="B11" r:id="rId10"/>
     <hyperlink ref="B10" r:id="rId11"/>
+    <hyperlink ref="B18" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated resistors and capacitors on BOM
</commit_message>
<xml_diff>
--- a/Notes/Pong.0 BOM.xlsx
+++ b/Notes/Pong.0 BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24240" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="24240" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Electronics" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="127">
   <si>
     <t>Mfg Part #</t>
   </si>
@@ -66,9 +66,6 @@
     <t>DigiKey</t>
   </si>
   <si>
-    <t>GRM319R71H104KA01D</t>
-  </si>
-  <si>
     <t>Used for Power Input/Output filtering and Decoupling</t>
   </si>
   <si>
@@ -132,24 +129,12 @@
     <t>TPS61240DRVT</t>
   </si>
   <si>
-    <t>5V 0.45A Boost Regulator</t>
-  </si>
-  <si>
     <t>6-WDFN</t>
   </si>
   <si>
     <t>5V Power for LEDs and Drivers</t>
   </si>
   <si>
-    <t>64 LED Driver</t>
-  </si>
-  <si>
-    <t>Capacitor Aluminum 10uF</t>
-  </si>
-  <si>
-    <t>Level Translator</t>
-  </si>
-  <si>
     <t>NVT2006PW,118</t>
   </si>
   <si>
@@ -186,9 +171,6 @@
     <t>CC2500RTKR</t>
   </si>
   <si>
-    <t>RF Transceiver</t>
-  </si>
-  <si>
     <t>20-VFQFN</t>
   </si>
   <si>
@@ -198,9 +180,6 @@
     <t>ATXMEGA16A4U-AUR</t>
   </si>
   <si>
-    <t>Atmel AVR XMEGA16A4U</t>
-  </si>
-  <si>
     <t>ABM8G-26.000MHZ-4Y-T3</t>
   </si>
   <si>
@@ -219,9 +198,6 @@
     <t>BQ24163RGET</t>
   </si>
   <si>
-    <t>Battery Manager/Charger</t>
-  </si>
-  <si>
     <t>0805</t>
   </si>
   <si>
@@ -234,7 +210,196 @@
     <t>6-TSOP</t>
   </si>
   <si>
-    <t>USB ESD Protection</t>
+    <t>Capacitor Ceramic 0.01uF</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>Resistor 560 Ohm</t>
+  </si>
+  <si>
+    <t>R13, R14, R15, R16, R18, R19, R20, R21</t>
+  </si>
+  <si>
+    <t>RX0, RX1, RX2, RX3, RX4, RX5, RX6, RX7, RS1, RS2, RS3, RS4, RS5, RS6, RY0, RY1, RY2, RY3</t>
+  </si>
+  <si>
+    <t>Resistor 1k</t>
+  </si>
+  <si>
+    <t>Resistor 10k</t>
+  </si>
+  <si>
+    <t>R5, R6, R7, R9, R10, R11, R12, R22, R24, R26, R27, R28</t>
+  </si>
+  <si>
+    <t>Resistor 100k</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>Resisitor 200k</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>Resistor 470k</t>
+  </si>
+  <si>
+    <t>RSMP0, RSMP1, RSMP2, RSMP3</t>
+  </si>
+  <si>
+    <t>Resistor 1M</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>C14, C16, C18, C43, C45, C46, C47, C52, C53, C54, C55, C56, C57, C59, C60</t>
+  </si>
+  <si>
+    <t>C22, C23, C24, C25, C26, C27, C28, C29, C30, C31, C32, C33, C34, C35, C36, C37, C38, C39, C40, C41</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 1nF</t>
+  </si>
+  <si>
+    <t>C8, C13, C15, C17, C44, C51, C58</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 15pF</t>
+  </si>
+  <si>
+    <t>C49, C50</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 1uF</t>
+  </si>
+  <si>
+    <t>C2, C3, C6, C9, C19, C20, C48</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 2.2uF</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 4.7nF</t>
+  </si>
+  <si>
+    <t>C1, CS0, CS1, CS2, CS3</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 4.7uF</t>
+  </si>
+  <si>
+    <t>C4, C5, C11, C12</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ103V</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ561V</t>
+  </si>
+  <si>
+    <t>Cheaper to buy 5000</t>
+  </si>
+  <si>
+    <t>MCR03EZP5J102</t>
+  </si>
+  <si>
+    <t>Cheaper to buy 10000</t>
+  </si>
+  <si>
+    <t>RC1608J104CS</t>
+  </si>
+  <si>
+    <t>RC1608J204CS</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF4703V</t>
+  </si>
+  <si>
+    <t>RC1608J105CS</t>
+  </si>
+  <si>
+    <t>C1608X7S0J106M080AC</t>
+  </si>
+  <si>
+    <t>Capacitor Ceramic 10uF</t>
+  </si>
+  <si>
+    <t>C1608X7S1A475M080AC</t>
+  </si>
+  <si>
+    <t>LMK107B7225KA-T</t>
+  </si>
+  <si>
+    <t>LMK107B7105KA-T</t>
+  </si>
+  <si>
+    <t>CL10B104KO8NNNC</t>
+  </si>
+  <si>
+    <t>CL10B103MB8NCNC</t>
+  </si>
+  <si>
+    <t>CL10B472KB8SFNC</t>
+  </si>
+  <si>
+    <t>CL10B102KB8SFNC</t>
+  </si>
+  <si>
+    <t>CL10C150JB8NCNC</t>
+  </si>
+  <si>
+    <t>AS1119-BWLT</t>
+  </si>
+  <si>
+    <t>36-WLCSP</t>
+  </si>
+  <si>
+    <t>LI Battery</t>
+  </si>
+  <si>
+    <t>W25X20CLSNIG</t>
+  </si>
+  <si>
+    <t>8-SOIC</t>
+  </si>
+  <si>
+    <t>IC Boost Regulator 5V 0.45A</t>
+  </si>
+  <si>
+    <t>IC 64 LED Driver</t>
+  </si>
+  <si>
+    <t>IC LED Matrix Driver</t>
+  </si>
+  <si>
+    <t>IC RF Transceiver</t>
+  </si>
+  <si>
+    <t>IC Battery Manager/Charger</t>
+  </si>
+  <si>
+    <t>IC USB ESD Protection</t>
+  </si>
+  <si>
+    <t>IC Flash Memory 2Mbit</t>
+  </si>
+  <si>
+    <t>IC Atmel AVR XMEGA16A4U</t>
+  </si>
+  <si>
+    <t>IC Level Translator</t>
   </si>
 </sst>
 </file>
@@ -245,7 +410,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +513,24 @@
       <color theme="1"/>
       <name val="Lucida Sans Unicode"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Lucida Sans Unicode"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1" tint="0.14996795556505021"/>
+      <name val="Lucida Sans Unicode"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Lucida Sans Unicode"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -391,7 +574,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -478,6 +661,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1011,8 +1223,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A4:L199" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="A4:L199"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A4:L214" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A4:L214"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Description" dataDxfId="23"/>
     <tableColumn id="2" name="Mfg Part #" dataDxfId="22"/>
@@ -1345,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L199"/>
+  <dimension ref="A1:L214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1369,18 +1581,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="A1" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
       <c r="K1" s="8" t="s">
         <v>4</v>
       </c>
@@ -1389,18 +1601,18 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
+      <c r="A2" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
@@ -1409,16 +1621,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="29">
-        <f>SUM(J5:J199)</f>
-        <v>10430.664999999999</v>
+        <f>SUM(J5:J214)</f>
+        <v>15209.26</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="29">
         <f>B3/Goal</f>
-        <v>20.861329999999999</v>
+        <v>30.418520000000001</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -1439,7 +1651,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -1468,10 +1680,10 @@
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>10</v>
@@ -1494,7 +1706,7 @@
         <v>2.0038999999999998</v>
       </c>
       <c r="J5" s="24">
-        <f>SUM(I5*H5)</f>
+        <f t="shared" ref="J5:J11" si="0">SUM(I5*H5)</f>
         <v>1001.9499999999999</v>
       </c>
       <c r="K5" s="19"/>
@@ -1502,13 +1714,13 @@
     </row>
     <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="19" t="s">
@@ -1528,764 +1740,1038 @@
         <v>0.49</v>
       </c>
       <c r="J6" s="24">
-        <f>SUM(I6*H6)</f>
+        <f t="shared" si="0"/>
         <v>245</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="19"/>
       <c r="F7" s="17"/>
       <c r="G7" s="15">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="H7" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>23500</v>
+        <v>32000</v>
       </c>
       <c r="I7" s="18">
         <v>0.03</v>
       </c>
       <c r="J7" s="24">
-        <f>SUM(I7*H7)</f>
-        <v>705</v>
+        <f t="shared" si="0"/>
+        <v>960</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:12" ht="27" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="15">
+    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="36">
+        <v>6750</v>
+      </c>
+      <c r="G8" s="37">
         <v>2</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="38">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>1000</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="24">
-        <f t="shared" ref="J8:J68" si="0">SUM(I8*H8)</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" s="19"/>
-    </row>
-    <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="23">
-        <v>1206</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="19" t="s">
+      <c r="I8" s="39">
+        <v>3.0899999999999999E-3</v>
+      </c>
+      <c r="J8" s="40">
+        <f t="shared" si="0"/>
+        <v>3.09</v>
+      </c>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="17">
-        <v>425577</v>
-      </c>
-      <c r="G9" s="15">
-        <v>30</v>
-      </c>
-      <c r="H9" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>15000</v>
-      </c>
-      <c r="I9" s="18">
-        <v>2.01E-2</v>
-      </c>
-      <c r="J9" s="24">
+      <c r="F9" s="36">
+        <v>24000</v>
+      </c>
+      <c r="G9" s="37">
+        <v>20</v>
+      </c>
+      <c r="H9" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>10000</v>
+      </c>
+      <c r="I9" s="39">
+        <v>2.3700000000000001E-3</v>
+      </c>
+      <c r="J9" s="40">
         <f t="shared" si="0"/>
-        <v>301.5</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="19"/>
+        <v>23.700000000000003</v>
+      </c>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="19" t="s">
+      <c r="A10" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="17">
-        <v>43194</v>
-      </c>
-      <c r="G10" s="15">
-        <v>1</v>
-      </c>
-      <c r="H10" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I10" s="18">
-        <v>4.3700000000000003E-2</v>
-      </c>
-      <c r="J10" s="24">
+      <c r="F10" s="36">
+        <v>8862</v>
+      </c>
+      <c r="G10" s="37">
+        <v>5</v>
+      </c>
+      <c r="H10" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>2500</v>
+      </c>
+      <c r="I10" s="39">
+        <v>6.1799999999999997E-3</v>
+      </c>
+      <c r="J10" s="40">
         <f t="shared" si="0"/>
-        <v>21.85</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="19"/>
+        <v>15.45</v>
+      </c>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="17">
-        <v>94327</v>
-      </c>
-      <c r="G11" s="15">
+      <c r="F11" s="36">
+        <v>7910</v>
+      </c>
+      <c r="G11" s="37">
         <v>1</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="38">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>500</v>
       </c>
-      <c r="I11" s="18">
-        <v>4.3700000000000003E-2</v>
-      </c>
-      <c r="J11" s="24">
+      <c r="I11" s="39">
+        <v>2.7799999999999999E-3</v>
+      </c>
+      <c r="J11" s="40">
         <f t="shared" si="0"/>
-        <v>21.85</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="19"/>
-    </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>1.39</v>
+      </c>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="19" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="17">
+        <v>3308000</v>
+      </c>
+      <c r="G12" s="15">
+        <v>15</v>
+      </c>
+      <c r="H12" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>7500</v>
+      </c>
+      <c r="I12" s="18">
+        <v>3.5899999999999999E-3</v>
+      </c>
+      <c r="J12" s="24">
+        <f t="shared" ref="J12:J83" si="1">SUM(I12*H12)</f>
+        <v>26.925000000000001</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="36">
+        <v>76000</v>
+      </c>
+      <c r="G13" s="37">
+        <v>7</v>
+      </c>
+      <c r="H13" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>3500</v>
+      </c>
+      <c r="I13" s="39">
+        <v>7.8200000000000006E-3</v>
+      </c>
+      <c r="J13" s="40">
+        <f t="shared" ref="J13:J23" si="2">SUM(I13*H13)</f>
+        <v>27.37</v>
+      </c>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="36">
+        <v>217168</v>
+      </c>
+      <c r="G14" s="37">
+        <v>1</v>
+      </c>
+      <c r="H14" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I14" s="39">
+        <v>3.8519999999999999E-2</v>
+      </c>
+      <c r="J14" s="40">
+        <f t="shared" si="2"/>
+        <v>19.259999999999998</v>
+      </c>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="42">
+        <v>1179</v>
+      </c>
+      <c r="G15" s="37">
+        <v>4</v>
+      </c>
+      <c r="H15" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>2000</v>
+      </c>
+      <c r="I15" s="39">
+        <v>6.1199999999999997E-2</v>
+      </c>
+      <c r="J15" s="40">
+        <f t="shared" si="2"/>
+        <v>122.39999999999999</v>
+      </c>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="26"/>
+      <c r="E16" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="17">
+        <v>4000</v>
+      </c>
+      <c r="G16" s="15">
+        <v>7</v>
+      </c>
+      <c r="H16" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>3500</v>
+      </c>
+      <c r="I16" s="18">
+        <v>0.26812999999999998</v>
+      </c>
+      <c r="J16" s="24">
+        <f t="shared" si="2"/>
+        <v>938.45499999999993</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="27"/>
+      <c r="E17" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="36">
+        <v>155000</v>
+      </c>
+      <c r="G17" s="37">
+        <v>8</v>
+      </c>
+      <c r="H17" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>4000</v>
+      </c>
+      <c r="I17" s="39">
+        <v>1.5200000000000001E-3</v>
+      </c>
+      <c r="J17" s="40">
+        <f t="shared" si="2"/>
+        <v>6.08</v>
+      </c>
+      <c r="K17" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="L17" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="36">
+        <v>1365000</v>
+      </c>
+      <c r="G18" s="37">
+        <v>18</v>
+      </c>
+      <c r="H18" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>9000</v>
+      </c>
+      <c r="I18" s="39">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="J18" s="40">
+        <f t="shared" si="2"/>
+        <v>10.799999999999999</v>
+      </c>
+      <c r="K18" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="L18" s="35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="36">
+        <v>8283494</v>
+      </c>
+      <c r="G19" s="37">
+        <v>12</v>
+      </c>
+      <c r="H19" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>6000</v>
+      </c>
+      <c r="I19" s="39">
+        <v>2.5600000000000002E-3</v>
+      </c>
+      <c r="J19" s="40">
+        <f t="shared" si="2"/>
+        <v>15.360000000000001</v>
+      </c>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="36">
+        <v>20673</v>
+      </c>
+      <c r="G20" s="37">
+        <v>1</v>
+      </c>
+      <c r="H20" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I20" s="39">
+        <v>2.7399999999999998E-3</v>
+      </c>
+      <c r="J20" s="40">
+        <f t="shared" si="2"/>
+        <v>1.3699999999999999</v>
+      </c>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="36">
+        <v>20000</v>
+      </c>
+      <c r="G21" s="37">
+        <v>1</v>
+      </c>
+      <c r="H21" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I21" s="39">
+        <v>2.7399999999999998E-3</v>
+      </c>
+      <c r="J21" s="40">
+        <f t="shared" si="2"/>
+        <v>1.3699999999999999</v>
+      </c>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="27"/>
+      <c r="E22" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="36">
+        <v>299269</v>
+      </c>
+      <c r="G22" s="37">
+        <v>4</v>
+      </c>
+      <c r="H22" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>2000</v>
+      </c>
+      <c r="I22" s="39">
+        <v>3.8400000000000001E-3</v>
+      </c>
+      <c r="J22" s="40">
+        <f t="shared" si="2"/>
+        <v>7.6800000000000006</v>
+      </c>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="27"/>
+      <c r="E23" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="36">
+        <v>12666</v>
+      </c>
+      <c r="G23" s="37">
+        <v>1</v>
+      </c>
+      <c r="H23" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I23" s="39">
+        <v>2.7399999999999998E-3</v>
+      </c>
+      <c r="J23" s="40">
+        <f t="shared" si="2"/>
+        <v>1.3699999999999999</v>
+      </c>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="17">
+        <v>43194</v>
+      </c>
+      <c r="G24" s="15">
+        <v>1</v>
+      </c>
+      <c r="H24" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I24" s="18">
+        <v>4.3700000000000003E-2</v>
+      </c>
+      <c r="J24" s="24">
+        <f t="shared" si="1"/>
+        <v>21.85</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" s="19"/>
+    </row>
+    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="17">
+        <v>94327</v>
+      </c>
+      <c r="G25" s="15">
+        <v>1</v>
+      </c>
+      <c r="H25" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I25" s="18">
+        <v>4.3700000000000003E-2</v>
+      </c>
+      <c r="J25" s="24">
+        <f t="shared" si="1"/>
+        <v>21.85</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="L25" s="19"/>
+    </row>
+    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="17">
         <v>51750</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G26" s="15">
         <v>1</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H26" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>500</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I26" s="18">
         <v>0.9425</v>
       </c>
-      <c r="J12" s="24">
-        <f t="shared" si="0"/>
+      <c r="J26" s="24">
+        <f t="shared" si="1"/>
         <v>471.25</v>
       </c>
-      <c r="K12" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="19"/>
-    </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="22" t="s">
+      <c r="K26" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L26" s="19"/>
+    </row>
+    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="17">
+        <v>12727</v>
+      </c>
+      <c r="G27" s="15">
+        <v>1</v>
+      </c>
+      <c r="H27" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I27" s="18">
+        <v>3.7223600000000001</v>
+      </c>
+      <c r="J27" s="24">
+        <f t="shared" si="1"/>
+        <v>1861.18</v>
+      </c>
+      <c r="K27" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="L27" s="19"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="27"/>
+      <c r="E28" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="36">
+        <v>2326</v>
+      </c>
+      <c r="G28" s="37">
+        <v>1</v>
+      </c>
+      <c r="H28" s="38">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I28" s="39">
+        <v>5.7294200000000002</v>
+      </c>
+      <c r="J28" s="40">
+        <f>SUM(I28*H28)</f>
+        <v>2864.71</v>
+      </c>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+    </row>
+    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="17">
+        <v>5213</v>
+      </c>
+      <c r="G29" s="15">
+        <v>1</v>
+      </c>
+      <c r="H29" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I29" s="18">
+        <v>0.83160000000000001</v>
+      </c>
+      <c r="J29" s="24">
+        <f t="shared" si="1"/>
+        <v>415.8</v>
+      </c>
+      <c r="K29" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="19" t="s">
+      <c r="L29" s="19"/>
+    </row>
+    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="23"/>
+      <c r="E30" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="17">
-        <v>12727</v>
-      </c>
-      <c r="G13" s="15">
-        <v>3</v>
-      </c>
-      <c r="H13" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>1500</v>
-      </c>
-      <c r="I13" s="18">
-        <v>3.1905899999999998</v>
-      </c>
-      <c r="J13" s="24">
-        <f t="shared" si="0"/>
-        <v>4785.8849999999993</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="L13" s="19"/>
-    </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="F30" s="17">
+        <v>15533</v>
+      </c>
+      <c r="G30" s="15">
+        <v>1</v>
+      </c>
+      <c r="H30" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>500</v>
+      </c>
+      <c r="I30" s="18">
+        <v>1.56</v>
+      </c>
+      <c r="J30" s="24">
+        <f t="shared" si="1"/>
+        <v>780</v>
+      </c>
+      <c r="K30" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="23" t="s">
+      <c r="L30" s="19"/>
+    </row>
+    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="19" t="s">
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="17">
-        <v>5213</v>
-      </c>
-      <c r="G14" s="15">
+      <c r="F31" s="17">
+        <v>6517</v>
+      </c>
+      <c r="G31" s="15">
         <v>1</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H31" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>500</v>
       </c>
-      <c r="I14" s="18">
-        <v>0.83160000000000001</v>
-      </c>
-      <c r="J14" s="24">
-        <f t="shared" si="0"/>
-        <v>415.8</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="L14" s="19"/>
-    </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="I31" s="18">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="J31" s="24">
+        <f t="shared" si="1"/>
+        <v>256.5</v>
+      </c>
+      <c r="K31" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="19" t="s">
+      <c r="L31" s="19"/>
+    </row>
+    <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="23"/>
+      <c r="E32" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="17">
-        <v>15533</v>
-      </c>
-      <c r="G15" s="15">
+      <c r="F32" s="17">
+        <v>706</v>
+      </c>
+      <c r="G32" s="15">
         <v>1</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H32" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
         <v>500</v>
       </c>
-      <c r="I15" s="18">
-        <v>1.56</v>
-      </c>
-      <c r="J15" s="24">
-        <f t="shared" si="0"/>
-        <v>780</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="L15" s="19"/>
-    </row>
-    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="17">
-        <v>6517</v>
-      </c>
-      <c r="G16" s="15">
-        <v>1</v>
-      </c>
-      <c r="H16" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I16" s="18">
-        <v>0.51300000000000001</v>
-      </c>
-      <c r="J16" s="24">
-        <f t="shared" si="0"/>
-        <v>256.5</v>
-      </c>
-      <c r="K16" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="L16" s="19"/>
-    </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="17">
-        <v>706</v>
-      </c>
-      <c r="G17" s="15">
-        <v>1</v>
-      </c>
-      <c r="H17" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I17" s="18">
+      <c r="I32" s="18">
         <v>2.6324999999999998</v>
       </c>
-      <c r="J17" s="24">
-        <f t="shared" si="0"/>
+      <c r="J32" s="24">
+        <f t="shared" si="1"/>
         <v>1316.25</v>
-      </c>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-    </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="17">
-        <v>8164</v>
-      </c>
-      <c r="G18" s="15">
-        <v>1</v>
-      </c>
-      <c r="H18" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>500</v>
-      </c>
-      <c r="I18" s="18">
-        <v>0.21565999999999999</v>
-      </c>
-      <c r="J18" s="24">
-        <f t="shared" si="0"/>
-        <v>107.83</v>
-      </c>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-    </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-    </row>
-    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-    </row>
-    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-    </row>
-    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-    </row>
-    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-    </row>
-    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-    </row>
-    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="18"/>
-      <c r="J25" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-    </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="18"/>
-      <c r="J26" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-    </row>
-    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="18"/>
-      <c r="J27" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-    </row>
-    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-    </row>
-    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-    </row>
-    <row r="30" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-    </row>
-    <row r="31" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="18"/>
-      <c r="J31" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-    </row>
-    <row r="32" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="25">
-        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="18"/>
-      <c r="J32" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
       <c r="K32" s="19"/>
       <c r="L32" s="19"/>
     </row>
     <row r="33" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="23"/>
+      <c r="A33" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>62</v>
+      </c>
       <c r="D33" s="23"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="15"/>
+      <c r="E33" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="17">
+        <v>8164</v>
+      </c>
+      <c r="G33" s="15">
+        <v>1</v>
+      </c>
       <c r="H33" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="18"/>
+        <v>500</v>
+      </c>
+      <c r="I33" s="18">
+        <v>0.21565999999999999</v>
+      </c>
       <c r="J33" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>107.83</v>
       </c>
       <c r="K33" s="19"/>
       <c r="L33" s="19"/>
     </row>
     <row r="34" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="20"/>
+      <c r="A34" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="22"/>
       <c r="C34" s="23"/>
       <c r="D34" s="23"/>
       <c r="E34" s="19"/>
       <c r="F34" s="17"/>
-      <c r="G34" s="15"/>
+      <c r="G34" s="15">
+        <v>1</v>
+      </c>
       <c r="H34" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="18"/>
+        <v>500</v>
+      </c>
+      <c r="I34" s="18">
+        <v>7</v>
+      </c>
       <c r="J34" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>3500</v>
       </c>
       <c r="K34" s="19"/>
       <c r="L34" s="19"/>
     </row>
     <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="23"/>
+      <c r="A35" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>117</v>
+      </c>
       <c r="D35" s="23"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="15"/>
+      <c r="E35" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="17">
+        <v>7531</v>
+      </c>
+      <c r="G35" s="15">
+        <v>1</v>
+      </c>
       <c r="H35" s="25">
         <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="18"/>
+        <v>500</v>
+      </c>
+      <c r="I35" s="18">
+        <v>0.32604</v>
+      </c>
       <c r="J35" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>163.02000000000001</v>
       </c>
       <c r="K35" s="19"/>
       <c r="L35" s="19"/>
@@ -2304,7 +2790,7 @@
       </c>
       <c r="I36" s="18"/>
       <c r="J36" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K36" s="19"/>
@@ -2312,9 +2798,9 @@
     </row>
     <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
       <c r="E37" s="19"/>
       <c r="F37" s="17"/>
       <c r="G37" s="15"/>
@@ -2324,7 +2810,7 @@
       </c>
       <c r="I37" s="18"/>
       <c r="J37" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K37" s="19"/>
@@ -2332,7 +2818,7 @@
     </row>
     <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
-      <c r="B38" s="20"/>
+      <c r="B38" s="22"/>
       <c r="C38" s="23"/>
       <c r="D38" s="23"/>
       <c r="E38" s="19"/>
@@ -2344,7 +2830,7 @@
       </c>
       <c r="I38" s="18"/>
       <c r="J38" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K38" s="19"/>
@@ -2352,7 +2838,7 @@
     </row>
     <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
-      <c r="B39" s="20"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="23"/>
       <c r="D39" s="23"/>
       <c r="E39" s="19"/>
@@ -2364,7 +2850,7 @@
       </c>
       <c r="I39" s="18"/>
       <c r="J39" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K39" s="19"/>
@@ -2384,7 +2870,7 @@
       </c>
       <c r="I40" s="18"/>
       <c r="J40" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K40" s="19"/>
@@ -2404,7 +2890,7 @@
       </c>
       <c r="I41" s="18"/>
       <c r="J41" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K41" s="19"/>
@@ -2424,7 +2910,7 @@
       </c>
       <c r="I42" s="18"/>
       <c r="J42" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K42" s="19"/>
@@ -2444,7 +2930,7 @@
       </c>
       <c r="I43" s="18"/>
       <c r="J43" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K43" s="19"/>
@@ -2464,7 +2950,7 @@
       </c>
       <c r="I44" s="18"/>
       <c r="J44" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K44" s="19"/>
@@ -2484,7 +2970,7 @@
       </c>
       <c r="I45" s="18"/>
       <c r="J45" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K45" s="19"/>
@@ -2504,7 +2990,7 @@
       </c>
       <c r="I46" s="18"/>
       <c r="J46" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K46" s="19"/>
@@ -2524,7 +3010,7 @@
       </c>
       <c r="I47" s="18"/>
       <c r="J47" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K47" s="19"/>
@@ -2544,7 +3030,7 @@
       </c>
       <c r="I48" s="18"/>
       <c r="J48" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K48" s="19"/>
@@ -2564,7 +3050,7 @@
       </c>
       <c r="I49" s="18"/>
       <c r="J49" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K49" s="19"/>
@@ -2584,7 +3070,7 @@
       </c>
       <c r="I50" s="18"/>
       <c r="J50" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K50" s="19"/>
@@ -2604,7 +3090,7 @@
       </c>
       <c r="I51" s="18"/>
       <c r="J51" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K51" s="19"/>
@@ -2624,7 +3110,7 @@
       </c>
       <c r="I52" s="18"/>
       <c r="J52" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K52" s="19"/>
@@ -2644,7 +3130,7 @@
       </c>
       <c r="I53" s="18"/>
       <c r="J53" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K53" s="19"/>
@@ -2664,7 +3150,7 @@
       </c>
       <c r="I54" s="18"/>
       <c r="J54" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K54" s="19"/>
@@ -2684,7 +3170,7 @@
       </c>
       <c r="I55" s="18"/>
       <c r="J55" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K55" s="19"/>
@@ -2704,7 +3190,7 @@
       </c>
       <c r="I56" s="18"/>
       <c r="J56" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K56" s="19"/>
@@ -2724,7 +3210,7 @@
       </c>
       <c r="I57" s="18"/>
       <c r="J57" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K57" s="19"/>
@@ -2744,7 +3230,7 @@
       </c>
       <c r="I58" s="18"/>
       <c r="J58" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K58" s="19"/>
@@ -2764,7 +3250,7 @@
       </c>
       <c r="I59" s="18"/>
       <c r="J59" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K59" s="19"/>
@@ -2784,7 +3270,7 @@
       </c>
       <c r="I60" s="18"/>
       <c r="J60" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K60" s="19"/>
@@ -2804,7 +3290,7 @@
       </c>
       <c r="I61" s="18"/>
       <c r="J61" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K61" s="19"/>
@@ -2824,7 +3310,7 @@
       </c>
       <c r="I62" s="18"/>
       <c r="J62" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K62" s="19"/>
@@ -2844,7 +3330,7 @@
       </c>
       <c r="I63" s="18"/>
       <c r="J63" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K63" s="19"/>
@@ -2864,7 +3350,7 @@
       </c>
       <c r="I64" s="18"/>
       <c r="J64" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K64" s="19"/>
@@ -2884,7 +3370,7 @@
       </c>
       <c r="I65" s="18"/>
       <c r="J65" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K65" s="19"/>
@@ -2904,7 +3390,7 @@
       </c>
       <c r="I66" s="18"/>
       <c r="J66" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K66" s="19"/>
@@ -2924,7 +3410,7 @@
       </c>
       <c r="I67" s="18"/>
       <c r="J67" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K67" s="19"/>
@@ -2944,7 +3430,7 @@
       </c>
       <c r="I68" s="18"/>
       <c r="J68" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K68" s="19"/>
@@ -2964,7 +3450,7 @@
       </c>
       <c r="I69" s="18"/>
       <c r="J69" s="24">
-        <f t="shared" ref="J69:J132" si="1">SUM(I69*H69)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K69" s="19"/>
@@ -3264,7 +3750,7 @@
       </c>
       <c r="I84" s="18"/>
       <c r="J84" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J84:J147" si="3">SUM(I84*H84)</f>
         <v>0</v>
       </c>
       <c r="K84" s="19"/>
@@ -3284,7 +3770,7 @@
       </c>
       <c r="I85" s="18"/>
       <c r="J85" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K85" s="19"/>
@@ -3304,7 +3790,7 @@
       </c>
       <c r="I86" s="18"/>
       <c r="J86" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K86" s="19"/>
@@ -3324,7 +3810,7 @@
       </c>
       <c r="I87" s="18"/>
       <c r="J87" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K87" s="19"/>
@@ -3344,7 +3830,7 @@
       </c>
       <c r="I88" s="18"/>
       <c r="J88" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K88" s="19"/>
@@ -3364,7 +3850,7 @@
       </c>
       <c r="I89" s="18"/>
       <c r="J89" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K89" s="19"/>
@@ -3384,7 +3870,7 @@
       </c>
       <c r="I90" s="18"/>
       <c r="J90" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K90" s="19"/>
@@ -3404,7 +3890,7 @@
       </c>
       <c r="I91" s="18"/>
       <c r="J91" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K91" s="19"/>
@@ -3424,7 +3910,7 @@
       </c>
       <c r="I92" s="18"/>
       <c r="J92" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K92" s="19"/>
@@ -3444,7 +3930,7 @@
       </c>
       <c r="I93" s="18"/>
       <c r="J93" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K93" s="19"/>
@@ -3464,7 +3950,7 @@
       </c>
       <c r="I94" s="18"/>
       <c r="J94" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K94" s="19"/>
@@ -3484,7 +3970,7 @@
       </c>
       <c r="I95" s="18"/>
       <c r="J95" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K95" s="19"/>
@@ -3504,7 +3990,7 @@
       </c>
       <c r="I96" s="18"/>
       <c r="J96" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K96" s="19"/>
@@ -3524,7 +4010,7 @@
       </c>
       <c r="I97" s="18"/>
       <c r="J97" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K97" s="19"/>
@@ -3544,7 +4030,7 @@
       </c>
       <c r="I98" s="18"/>
       <c r="J98" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K98" s="19"/>
@@ -3564,7 +4050,7 @@
       </c>
       <c r="I99" s="18"/>
       <c r="J99" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K99" s="19"/>
@@ -3584,7 +4070,7 @@
       </c>
       <c r="I100" s="18"/>
       <c r="J100" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K100" s="19"/>
@@ -3604,7 +4090,7 @@
       </c>
       <c r="I101" s="18"/>
       <c r="J101" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K101" s="19"/>
@@ -3624,7 +4110,7 @@
       </c>
       <c r="I102" s="18"/>
       <c r="J102" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K102" s="19"/>
@@ -3644,7 +4130,7 @@
       </c>
       <c r="I103" s="18"/>
       <c r="J103" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K103" s="19"/>
@@ -3664,7 +4150,7 @@
       </c>
       <c r="I104" s="18"/>
       <c r="J104" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K104" s="19"/>
@@ -3684,7 +4170,7 @@
       </c>
       <c r="I105" s="18"/>
       <c r="J105" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K105" s="19"/>
@@ -3704,7 +4190,7 @@
       </c>
       <c r="I106" s="18"/>
       <c r="J106" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K106" s="19"/>
@@ -3724,7 +4210,7 @@
       </c>
       <c r="I107" s="18"/>
       <c r="J107" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K107" s="19"/>
@@ -3744,7 +4230,7 @@
       </c>
       <c r="I108" s="18"/>
       <c r="J108" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K108" s="19"/>
@@ -3764,7 +4250,7 @@
       </c>
       <c r="I109" s="18"/>
       <c r="J109" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K109" s="19"/>
@@ -3784,7 +4270,7 @@
       </c>
       <c r="I110" s="18"/>
       <c r="J110" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K110" s="19"/>
@@ -3804,7 +4290,7 @@
       </c>
       <c r="I111" s="18"/>
       <c r="J111" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K111" s="19"/>
@@ -3824,7 +4310,7 @@
       </c>
       <c r="I112" s="18"/>
       <c r="J112" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K112" s="19"/>
@@ -3844,7 +4330,7 @@
       </c>
       <c r="I113" s="18"/>
       <c r="J113" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K113" s="19"/>
@@ -3864,7 +4350,7 @@
       </c>
       <c r="I114" s="18"/>
       <c r="J114" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K114" s="19"/>
@@ -3884,7 +4370,7 @@
       </c>
       <c r="I115" s="18"/>
       <c r="J115" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K115" s="19"/>
@@ -3904,7 +4390,7 @@
       </c>
       <c r="I116" s="18"/>
       <c r="J116" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K116" s="19"/>
@@ -3924,7 +4410,7 @@
       </c>
       <c r="I117" s="18"/>
       <c r="J117" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K117" s="19"/>
@@ -3944,7 +4430,7 @@
       </c>
       <c r="I118" s="18"/>
       <c r="J118" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K118" s="19"/>
@@ -3964,7 +4450,7 @@
       </c>
       <c r="I119" s="18"/>
       <c r="J119" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K119" s="19"/>
@@ -3984,7 +4470,7 @@
       </c>
       <c r="I120" s="18"/>
       <c r="J120" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K120" s="19"/>
@@ -4004,7 +4490,7 @@
       </c>
       <c r="I121" s="18"/>
       <c r="J121" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K121" s="19"/>
@@ -4024,7 +4510,7 @@
       </c>
       <c r="I122" s="18"/>
       <c r="J122" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K122" s="19"/>
@@ -4044,7 +4530,7 @@
       </c>
       <c r="I123" s="18"/>
       <c r="J123" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K123" s="19"/>
@@ -4064,7 +4550,7 @@
       </c>
       <c r="I124" s="18"/>
       <c r="J124" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K124" s="19"/>
@@ -4084,7 +4570,7 @@
       </c>
       <c r="I125" s="18"/>
       <c r="J125" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K125" s="19"/>
@@ -4104,7 +4590,7 @@
       </c>
       <c r="I126" s="18"/>
       <c r="J126" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K126" s="19"/>
@@ -4124,7 +4610,7 @@
       </c>
       <c r="I127" s="18"/>
       <c r="J127" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K127" s="19"/>
@@ -4144,7 +4630,7 @@
       </c>
       <c r="I128" s="18"/>
       <c r="J128" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K128" s="19"/>
@@ -4164,7 +4650,7 @@
       </c>
       <c r="I129" s="18"/>
       <c r="J129" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K129" s="19"/>
@@ -4184,7 +4670,7 @@
       </c>
       <c r="I130" s="18"/>
       <c r="J130" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K130" s="19"/>
@@ -4204,7 +4690,7 @@
       </c>
       <c r="I131" s="18"/>
       <c r="J131" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K131" s="19"/>
@@ -4224,7 +4710,7 @@
       </c>
       <c r="I132" s="18"/>
       <c r="J132" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K132" s="19"/>
@@ -4244,7 +4730,7 @@
       </c>
       <c r="I133" s="18"/>
       <c r="J133" s="24">
-        <f t="shared" ref="J133:J196" si="2">SUM(I133*H133)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K133" s="19"/>
@@ -4264,7 +4750,7 @@
       </c>
       <c r="I134" s="18"/>
       <c r="J134" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K134" s="19"/>
@@ -4284,7 +4770,7 @@
       </c>
       <c r="I135" s="18"/>
       <c r="J135" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K135" s="19"/>
@@ -4304,7 +4790,7 @@
       </c>
       <c r="I136" s="18"/>
       <c r="J136" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K136" s="19"/>
@@ -4324,7 +4810,7 @@
       </c>
       <c r="I137" s="18"/>
       <c r="J137" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K137" s="19"/>
@@ -4344,7 +4830,7 @@
       </c>
       <c r="I138" s="18"/>
       <c r="J138" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K138" s="19"/>
@@ -4364,7 +4850,7 @@
       </c>
       <c r="I139" s="18"/>
       <c r="J139" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K139" s="19"/>
@@ -4384,7 +4870,7 @@
       </c>
       <c r="I140" s="18"/>
       <c r="J140" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K140" s="19"/>
@@ -4404,7 +4890,7 @@
       </c>
       <c r="I141" s="18"/>
       <c r="J141" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K141" s="19"/>
@@ -4424,7 +4910,7 @@
       </c>
       <c r="I142" s="18"/>
       <c r="J142" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K142" s="19"/>
@@ -4444,7 +4930,7 @@
       </c>
       <c r="I143" s="18"/>
       <c r="J143" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K143" s="19"/>
@@ -4464,7 +4950,7 @@
       </c>
       <c r="I144" s="18"/>
       <c r="J144" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K144" s="19"/>
@@ -4484,7 +4970,7 @@
       </c>
       <c r="I145" s="18"/>
       <c r="J145" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K145" s="19"/>
@@ -4504,7 +4990,7 @@
       </c>
       <c r="I146" s="18"/>
       <c r="J146" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K146" s="19"/>
@@ -4524,7 +5010,7 @@
       </c>
       <c r="I147" s="18"/>
       <c r="J147" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K147" s="19"/>
@@ -4544,7 +5030,7 @@
       </c>
       <c r="I148" s="18"/>
       <c r="J148" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J148:J211" si="4">SUM(I148*H148)</f>
         <v>0</v>
       </c>
       <c r="K148" s="19"/>
@@ -4564,7 +5050,7 @@
       </c>
       <c r="I149" s="18"/>
       <c r="J149" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K149" s="19"/>
@@ -4584,7 +5070,7 @@
       </c>
       <c r="I150" s="18"/>
       <c r="J150" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K150" s="19"/>
@@ -4604,7 +5090,7 @@
       </c>
       <c r="I151" s="18"/>
       <c r="J151" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K151" s="19"/>
@@ -4624,7 +5110,7 @@
       </c>
       <c r="I152" s="18"/>
       <c r="J152" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K152" s="19"/>
@@ -4644,7 +5130,7 @@
       </c>
       <c r="I153" s="18"/>
       <c r="J153" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K153" s="19"/>
@@ -4664,7 +5150,7 @@
       </c>
       <c r="I154" s="18"/>
       <c r="J154" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K154" s="19"/>
@@ -4684,7 +5170,7 @@
       </c>
       <c r="I155" s="18"/>
       <c r="J155" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K155" s="19"/>
@@ -4704,7 +5190,7 @@
       </c>
       <c r="I156" s="18"/>
       <c r="J156" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K156" s="19"/>
@@ -4724,7 +5210,7 @@
       </c>
       <c r="I157" s="18"/>
       <c r="J157" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K157" s="19"/>
@@ -4744,7 +5230,7 @@
       </c>
       <c r="I158" s="18"/>
       <c r="J158" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K158" s="19"/>
@@ -4764,7 +5250,7 @@
       </c>
       <c r="I159" s="18"/>
       <c r="J159" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K159" s="19"/>
@@ -4784,7 +5270,7 @@
       </c>
       <c r="I160" s="18"/>
       <c r="J160" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K160" s="19"/>
@@ -4804,7 +5290,7 @@
       </c>
       <c r="I161" s="18"/>
       <c r="J161" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K161" s="19"/>
@@ -4824,7 +5310,7 @@
       </c>
       <c r="I162" s="18"/>
       <c r="J162" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K162" s="19"/>
@@ -4844,7 +5330,7 @@
       </c>
       <c r="I163" s="18"/>
       <c r="J163" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K163" s="19"/>
@@ -4864,7 +5350,7 @@
       </c>
       <c r="I164" s="18"/>
       <c r="J164" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K164" s="19"/>
@@ -4884,7 +5370,7 @@
       </c>
       <c r="I165" s="18"/>
       <c r="J165" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K165" s="19"/>
@@ -4904,7 +5390,7 @@
       </c>
       <c r="I166" s="18"/>
       <c r="J166" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K166" s="19"/>
@@ -4924,7 +5410,7 @@
       </c>
       <c r="I167" s="18"/>
       <c r="J167" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K167" s="19"/>
@@ -4944,7 +5430,7 @@
       </c>
       <c r="I168" s="18"/>
       <c r="J168" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K168" s="19"/>
@@ -4964,7 +5450,7 @@
       </c>
       <c r="I169" s="18"/>
       <c r="J169" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K169" s="19"/>
@@ -4984,7 +5470,7 @@
       </c>
       <c r="I170" s="18"/>
       <c r="J170" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K170" s="19"/>
@@ -5004,7 +5490,7 @@
       </c>
       <c r="I171" s="18"/>
       <c r="J171" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K171" s="19"/>
@@ -5024,7 +5510,7 @@
       </c>
       <c r="I172" s="18"/>
       <c r="J172" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K172" s="19"/>
@@ -5044,7 +5530,7 @@
       </c>
       <c r="I173" s="18"/>
       <c r="J173" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K173" s="19"/>
@@ -5064,7 +5550,7 @@
       </c>
       <c r="I174" s="18"/>
       <c r="J174" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K174" s="19"/>
@@ -5084,7 +5570,7 @@
       </c>
       <c r="I175" s="18"/>
       <c r="J175" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K175" s="19"/>
@@ -5104,7 +5590,7 @@
       </c>
       <c r="I176" s="18"/>
       <c r="J176" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K176" s="19"/>
@@ -5124,7 +5610,7 @@
       </c>
       <c r="I177" s="18"/>
       <c r="J177" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K177" s="19"/>
@@ -5144,7 +5630,7 @@
       </c>
       <c r="I178" s="18"/>
       <c r="J178" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K178" s="19"/>
@@ -5164,7 +5650,7 @@
       </c>
       <c r="I179" s="18"/>
       <c r="J179" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K179" s="19"/>
@@ -5184,7 +5670,7 @@
       </c>
       <c r="I180" s="18"/>
       <c r="J180" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K180" s="19"/>
@@ -5204,7 +5690,7 @@
       </c>
       <c r="I181" s="18"/>
       <c r="J181" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K181" s="19"/>
@@ -5224,7 +5710,7 @@
       </c>
       <c r="I182" s="18"/>
       <c r="J182" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K182" s="19"/>
@@ -5244,7 +5730,7 @@
       </c>
       <c r="I183" s="18"/>
       <c r="J183" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K183" s="19"/>
@@ -5264,7 +5750,7 @@
       </c>
       <c r="I184" s="18"/>
       <c r="J184" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K184" s="19"/>
@@ -5284,7 +5770,7 @@
       </c>
       <c r="I185" s="18"/>
       <c r="J185" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K185" s="19"/>
@@ -5304,7 +5790,7 @@
       </c>
       <c r="I186" s="18"/>
       <c r="J186" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K186" s="19"/>
@@ -5324,7 +5810,7 @@
       </c>
       <c r="I187" s="18"/>
       <c r="J187" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K187" s="19"/>
@@ -5344,7 +5830,7 @@
       </c>
       <c r="I188" s="18"/>
       <c r="J188" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K188" s="19"/>
@@ -5364,7 +5850,7 @@
       </c>
       <c r="I189" s="18"/>
       <c r="J189" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K189" s="19"/>
@@ -5384,7 +5870,7 @@
       </c>
       <c r="I190" s="18"/>
       <c r="J190" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K190" s="19"/>
@@ -5404,7 +5890,7 @@
       </c>
       <c r="I191" s="18"/>
       <c r="J191" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K191" s="19"/>
@@ -5424,7 +5910,7 @@
       </c>
       <c r="I192" s="18"/>
       <c r="J192" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K192" s="19"/>
@@ -5444,7 +5930,7 @@
       </c>
       <c r="I193" s="18"/>
       <c r="J193" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K193" s="19"/>
@@ -5464,7 +5950,7 @@
       </c>
       <c r="I194" s="18"/>
       <c r="J194" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K194" s="19"/>
@@ -5484,7 +5970,7 @@
       </c>
       <c r="I195" s="18"/>
       <c r="J195" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K195" s="19"/>
@@ -5504,7 +5990,7 @@
       </c>
       <c r="I196" s="18"/>
       <c r="J196" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K196" s="19"/>
@@ -5524,7 +6010,7 @@
       </c>
       <c r="I197" s="18"/>
       <c r="J197" s="24">
-        <f t="shared" ref="J197:J199" si="3">SUM(I197*H197)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K197" s="19"/>
@@ -5544,7 +6030,7 @@
       </c>
       <c r="I198" s="18"/>
       <c r="J198" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K198" s="19"/>
@@ -5564,11 +6050,311 @@
       </c>
       <c r="I199" s="18"/>
       <c r="J199" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K199" s="19"/>
       <c r="L199" s="19"/>
+    </row>
+    <row r="200" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A200" s="21"/>
+      <c r="B200" s="20"/>
+      <c r="C200" s="23"/>
+      <c r="D200" s="23"/>
+      <c r="E200" s="19"/>
+      <c r="F200" s="17"/>
+      <c r="G200" s="15"/>
+      <c r="H200" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I200" s="18"/>
+      <c r="J200" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K200" s="19"/>
+      <c r="L200" s="19"/>
+    </row>
+    <row r="201" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A201" s="21"/>
+      <c r="B201" s="20"/>
+      <c r="C201" s="23"/>
+      <c r="D201" s="23"/>
+      <c r="E201" s="19"/>
+      <c r="F201" s="17"/>
+      <c r="G201" s="15"/>
+      <c r="H201" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I201" s="18"/>
+      <c r="J201" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K201" s="19"/>
+      <c r="L201" s="19"/>
+    </row>
+    <row r="202" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A202" s="21"/>
+      <c r="B202" s="20"/>
+      <c r="C202" s="23"/>
+      <c r="D202" s="23"/>
+      <c r="E202" s="19"/>
+      <c r="F202" s="17"/>
+      <c r="G202" s="15"/>
+      <c r="H202" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I202" s="18"/>
+      <c r="J202" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K202" s="19"/>
+      <c r="L202" s="19"/>
+    </row>
+    <row r="203" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A203" s="21"/>
+      <c r="B203" s="20"/>
+      <c r="C203" s="23"/>
+      <c r="D203" s="23"/>
+      <c r="E203" s="19"/>
+      <c r="F203" s="17"/>
+      <c r="G203" s="15"/>
+      <c r="H203" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I203" s="18"/>
+      <c r="J203" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K203" s="19"/>
+      <c r="L203" s="19"/>
+    </row>
+    <row r="204" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A204" s="21"/>
+      <c r="B204" s="20"/>
+      <c r="C204" s="23"/>
+      <c r="D204" s="23"/>
+      <c r="E204" s="19"/>
+      <c r="F204" s="17"/>
+      <c r="G204" s="15"/>
+      <c r="H204" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I204" s="18"/>
+      <c r="J204" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K204" s="19"/>
+      <c r="L204" s="19"/>
+    </row>
+    <row r="205" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A205" s="21"/>
+      <c r="B205" s="20"/>
+      <c r="C205" s="23"/>
+      <c r="D205" s="23"/>
+      <c r="E205" s="19"/>
+      <c r="F205" s="17"/>
+      <c r="G205" s="15"/>
+      <c r="H205" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I205" s="18"/>
+      <c r="J205" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K205" s="19"/>
+      <c r="L205" s="19"/>
+    </row>
+    <row r="206" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A206" s="21"/>
+      <c r="B206" s="20"/>
+      <c r="C206" s="23"/>
+      <c r="D206" s="23"/>
+      <c r="E206" s="19"/>
+      <c r="F206" s="17"/>
+      <c r="G206" s="15"/>
+      <c r="H206" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I206" s="18"/>
+      <c r="J206" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K206" s="19"/>
+      <c r="L206" s="19"/>
+    </row>
+    <row r="207" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A207" s="21"/>
+      <c r="B207" s="20"/>
+      <c r="C207" s="23"/>
+      <c r="D207" s="23"/>
+      <c r="E207" s="19"/>
+      <c r="F207" s="17"/>
+      <c r="G207" s="15"/>
+      <c r="H207" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I207" s="18"/>
+      <c r="J207" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K207" s="19"/>
+      <c r="L207" s="19"/>
+    </row>
+    <row r="208" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A208" s="21"/>
+      <c r="B208" s="20"/>
+      <c r="C208" s="23"/>
+      <c r="D208" s="23"/>
+      <c r="E208" s="19"/>
+      <c r="F208" s="17"/>
+      <c r="G208" s="15"/>
+      <c r="H208" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I208" s="18"/>
+      <c r="J208" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K208" s="19"/>
+      <c r="L208" s="19"/>
+    </row>
+    <row r="209" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A209" s="21"/>
+      <c r="B209" s="20"/>
+      <c r="C209" s="23"/>
+      <c r="D209" s="23"/>
+      <c r="E209" s="19"/>
+      <c r="F209" s="17"/>
+      <c r="G209" s="15"/>
+      <c r="H209" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I209" s="18"/>
+      <c r="J209" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K209" s="19"/>
+      <c r="L209" s="19"/>
+    </row>
+    <row r="210" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A210" s="21"/>
+      <c r="B210" s="20"/>
+      <c r="C210" s="23"/>
+      <c r="D210" s="23"/>
+      <c r="E210" s="19"/>
+      <c r="F210" s="17"/>
+      <c r="G210" s="15"/>
+      <c r="H210" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I210" s="18"/>
+      <c r="J210" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K210" s="19"/>
+      <c r="L210" s="19"/>
+    </row>
+    <row r="211" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A211" s="21"/>
+      <c r="B211" s="20"/>
+      <c r="C211" s="23"/>
+      <c r="D211" s="23"/>
+      <c r="E211" s="19"/>
+      <c r="F211" s="17"/>
+      <c r="G211" s="15"/>
+      <c r="H211" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I211" s="18"/>
+      <c r="J211" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K211" s="19"/>
+      <c r="L211" s="19"/>
+    </row>
+    <row r="212" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A212" s="21"/>
+      <c r="B212" s="20"/>
+      <c r="C212" s="23"/>
+      <c r="D212" s="23"/>
+      <c r="E212" s="19"/>
+      <c r="F212" s="17"/>
+      <c r="G212" s="15"/>
+      <c r="H212" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I212" s="18"/>
+      <c r="J212" s="24">
+        <f t="shared" ref="J212:J214" si="5">SUM(I212*H212)</f>
+        <v>0</v>
+      </c>
+      <c r="K212" s="19"/>
+      <c r="L212" s="19"/>
+    </row>
+    <row r="213" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A213" s="21"/>
+      <c r="B213" s="20"/>
+      <c r="C213" s="23"/>
+      <c r="D213" s="23"/>
+      <c r="E213" s="19"/>
+      <c r="F213" s="17"/>
+      <c r="G213" s="15"/>
+      <c r="H213" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I213" s="18"/>
+      <c r="J213" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K213" s="19"/>
+      <c r="L213" s="19"/>
+    </row>
+    <row r="214" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A214" s="21"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="23"/>
+      <c r="D214" s="23"/>
+      <c r="E214" s="19"/>
+      <c r="F214" s="17"/>
+      <c r="G214" s="15"/>
+      <c r="H214" s="25">
+        <f>SUM(Table4[[#This Row],[Qty per board]]*Goal)</f>
+        <v>0</v>
+      </c>
+      <c r="I214" s="18"/>
+      <c r="J214" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K214" s="19"/>
+      <c r="L214" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5578,21 +6364,20 @@
   <hyperlinks>
     <hyperlink ref="A2:J2" r:id="rId1" display=" Projects and Stuff LLC - http://ww.projectsandstuff.com"/>
     <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B13" r:id="rId5"/>
-    <hyperlink ref="B14" r:id="rId6"/>
-    <hyperlink ref="B15" r:id="rId7"/>
-    <hyperlink ref="B16" r:id="rId8"/>
-    <hyperlink ref="B17" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B10" r:id="rId11"/>
-    <hyperlink ref="B18" r:id="rId12"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B27" r:id="rId4"/>
+    <hyperlink ref="B29" r:id="rId5"/>
+    <hyperlink ref="B30" r:id="rId6"/>
+    <hyperlink ref="B31" r:id="rId7"/>
+    <hyperlink ref="B32" r:id="rId8"/>
+    <hyperlink ref="B25" r:id="rId9"/>
+    <hyperlink ref="B24" r:id="rId10"/>
+    <hyperlink ref="B33" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5621,16 +6406,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="A1" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
       <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
@@ -5639,16 +6424,16 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="A2" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
@@ -5715,13 +6500,13 @@
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="C6" s="19" t="s">
         <v>30</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>31</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="15">
@@ -5739,7 +6524,7 @@
         <v>635</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J6" s="19"/>
     </row>

</xml_diff>